<commit_message>
feat: created film category and other tables
</commit_message>
<xml_diff>
--- a/cinema-database.xlsx
+++ b/cinema-database.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
   <si>
     <t>Id</t>
   </si>
@@ -81,6 +81,111 @@
   </si>
   <si>
     <t>Oyuncular</t>
+  </si>
+  <si>
+    <t>Açıklama</t>
+  </si>
+  <si>
+    <t>Süre</t>
+  </si>
+  <si>
+    <t>Yayın</t>
+  </si>
+  <si>
+    <t>Banner Image</t>
+  </si>
+  <si>
+    <t>Tanıtım</t>
+  </si>
+  <si>
+    <t>açıklama1</t>
+  </si>
+  <si>
+    <t>açıklama2</t>
+  </si>
+  <si>
+    <t>açıklama3</t>
+  </si>
+  <si>
+    <t>açıklama4</t>
+  </si>
+  <si>
+    <t>1.jpg</t>
+  </si>
+  <si>
+    <t>2.jpg</t>
+  </si>
+  <si>
+    <t>3.jpg</t>
+  </si>
+  <si>
+    <t>4.jpg</t>
+  </si>
+  <si>
+    <t>1.mp4</t>
+  </si>
+  <si>
+    <t>2.mp4</t>
+  </si>
+  <si>
+    <t>3.mp4</t>
+  </si>
+  <si>
+    <t>4.mp4</t>
+  </si>
+  <si>
+    <t>Doğum T.</t>
+  </si>
+  <si>
+    <t>Cinsiyet</t>
+  </si>
+  <si>
+    <t>Erkek</t>
+  </si>
+  <si>
+    <t>Kadın</t>
+  </si>
+  <si>
+    <t>Ülke</t>
+  </si>
+  <si>
+    <t>Türkiye</t>
+  </si>
+  <si>
+    <t>Amerika</t>
+  </si>
+  <si>
+    <t>Almanya</t>
+  </si>
+  <si>
+    <t>Rusya</t>
+  </si>
+  <si>
+    <t>Cem</t>
+  </si>
+  <si>
+    <t>Efe</t>
+  </si>
+  <si>
+    <t>Kaan</t>
+  </si>
+  <si>
+    <t>Toprak</t>
+  </si>
+  <si>
+    <t>Kategori</t>
+  </si>
+  <si>
+    <t>Korku</t>
+  </si>
+  <si>
+    <t>Romantik</t>
+  </si>
+  <si>
+    <t>Sevgi</t>
+  </si>
+  <si>
+    <t>Hüzün</t>
   </si>
 </sst>
 </file>
@@ -455,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,9 +572,10 @@
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -479,8 +585,23 @@
       <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2">
         <v>1</v>
@@ -488,8 +609,23 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2">
+        <v>120</v>
+      </c>
+      <c r="F2">
+        <v>2024</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3">
         <v>2</v>
@@ -497,8 +633,23 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3">
+        <v>111</v>
+      </c>
+      <c r="F3">
+        <v>2022</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4">
         <v>3</v>
@@ -506,8 +657,23 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <v>214</v>
+      </c>
+      <c r="F4">
+        <v>1998</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5">
         <v>4</v>
@@ -515,8 +681,23 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5">
+        <v>119</v>
+      </c>
+      <c r="F5">
+        <v>2004</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -529,8 +710,17 @@
       <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8">
         <v>1</v>
@@ -541,8 +731,17 @@
       <c r="D8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>1980</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9">
         <v>2</v>
@@ -553,8 +752,17 @@
       <c r="D9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>2000</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10">
         <v>3</v>
@@ -565,8 +773,17 @@
       <c r="D10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>1975</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11">
         <v>4</v>
@@ -577,8 +794,17 @@
       <c r="D11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>1961</v>
+      </c>
+      <c r="F11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -591,53 +817,160 @@
       <c r="D13" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>1980</v>
+      </c>
+      <c r="F14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="D15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>2000</v>
+      </c>
+      <c r="F15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16">
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>1975</v>
+      </c>
+      <c r="F16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17">
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
         <v>17</v>
+      </c>
+      <c r="E17">
+        <v>1961</v>
+      </c>
+      <c r="F17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>